<commit_message>
Added references, Modified schedule
</commit_message>
<xml_diff>
--- a/Schedule of Thesis.xlsx
+++ b/Schedule of Thesis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Start Date</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Doing</t>
+  </si>
+  <si>
+    <t>Mercado, Nel</t>
+  </si>
+  <si>
+    <t>Alcala, Michael</t>
+  </si>
+  <si>
+    <t>Garcia, Jasper</t>
   </si>
 </sst>
 </file>
@@ -635,7 +644,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1"/>
@@ -736,7 +745,9 @@
       <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="7">
+        <v>43319</v>
+      </c>
       <c r="C5" s="7">
         <v>43335</v>
       </c>
@@ -745,7 +756,9 @@
         <v>16</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="19.95" customHeight="1">
       <c r="A6" s="11" t="s">
@@ -762,7 +775,9 @@
         <v>1</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="F6" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="19.95" customHeight="1">
       <c r="A7" s="11" t="s">
@@ -779,85 +794,111 @@
         <v>1</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="19.95" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <v>43335</v>
+      </c>
       <c r="D8" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="19.95" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7">
+        <v>43335</v>
+      </c>
       <c r="D9" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="19.95" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7">
+        <v>43335</v>
+      </c>
       <c r="D10" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="19.95" customHeight="1">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7">
+        <v>43335</v>
+      </c>
       <c r="D11" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="19.95" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7">
+        <v>43335</v>
+      </c>
       <c r="D12" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="19.95" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7">
+        <v>43335</v>
+      </c>
       <c r="D13" s="8">
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="19.95" customHeight="1">
       <c r="A14" s="12" t="s">

</xml_diff>

<commit_message>
Added Sop and Bos
</commit_message>
<xml_diff>
--- a/Schedule of Thesis.xlsx
+++ b/Schedule of Thesis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Start Date</t>
   </si>
@@ -644,7 +644,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1"/>
@@ -774,7 +774,9 @@
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
         <v>1</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="13" t="s">
         <v>36</v>
       </c>
@@ -793,7 +795,9 @@
         <f ca="1">IF(ISBLANK(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)),0,IF(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1=0,"DEADLINE",OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1)-I1))</f>
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="F7" s="13" t="s">
         <v>30</v>
       </c>

</xml_diff>